<commit_message>
number of detections in the focal river
</commit_message>
<xml_diff>
--- a/Results_tables.xlsx
+++ b/Results_tables.xlsx
@@ -830,12 +830,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -847,19 +841,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
@@ -880,17 +865,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1214,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z9" sqref="Z9:Z10"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,166 +1247,166 @@
       <c r="A1" t="s">
         <v>63</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="Y1" s="2" t="s">
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="Y1" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2"/>
-      <c r="AF1" s="2"/>
-      <c r="AG1" s="2"/>
-      <c r="AH1" s="2"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="25"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
-      <c r="AE2" s="2"/>
-      <c r="AF2" s="2"/>
-      <c r="AG2" s="2"/>
-      <c r="AH2" s="2"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="Y2" s="25"/>
+      <c r="Z2" s="25"/>
+      <c r="AA2" s="25"/>
+      <c r="AB2" s="25"/>
+      <c r="AC2" s="25"/>
+      <c r="AD2" s="25"/>
+      <c r="AE2" s="25"/>
+      <c r="AF2" s="25"/>
+      <c r="AG2" s="25"/>
+      <c r="AH2" s="25"/>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21" t="s">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21" t="s">
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="U3" s="21"/>
-      <c r="V3" s="21"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="J4" s="22" t="s">
+      <c r="J4" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="K4" s="22" t="s">
+      <c r="K4" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="L4" s="22" t="s">
+      <c r="L4" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="M4" s="22" t="s">
+      <c r="M4" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="O4" s="22" t="s">
+      <c r="O4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="22" t="s">
+      <c r="P4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="22" t="s">
+      <c r="Q4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="R4" s="22" t="s">
+      <c r="R4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="S4" s="22"/>
-      <c r="T4" s="22" t="s">
+      <c r="S4" s="15"/>
+      <c r="T4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="U4" s="22" t="s">
+      <c r="U4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="V4" s="22" t="s">
+      <c r="V4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="Y4" s="25"/>
-      <c r="Z4" s="25" t="s">
+      <c r="Y4" s="18"/>
+      <c r="Z4" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="AA4" s="25" t="s">
+      <c r="AA4" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="AB4" s="25" t="s">
+      <c r="AB4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="AC4" s="25" t="s">
+      <c r="AC4" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="AD4" s="25" t="s">
+      <c r="AD4" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="AE4" s="25" t="s">
+      <c r="AE4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="AF4" s="25" t="s">
+      <c r="AF4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="AG4" s="25" t="s">
+      <c r="AG4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="AH4" s="25" t="s">
+      <c r="AH4" s="18" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1450,37 +1450,37 @@
       <c r="M5">
         <v>0</v>
       </c>
-      <c r="O5" s="23" t="s">
+      <c r="O5" s="16" t="s">
         <v>18</v>
       </c>
       <c r="Y5" t="s">
         <v>9</v>
       </c>
-      <c r="Z5" s="7">
+      <c r="Z5" s="5">
         <v>0.99</v>
       </c>
-      <c r="AA5" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB5" s="9">
+      <c r="AA5" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB5" s="6">
         <v>0.01</v>
       </c>
-      <c r="AC5" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD5" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AE5" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF5" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG5" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH5" s="3" t="s">
+      <c r="AC5" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD5" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE5" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF5" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG5" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH5" s="19" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1545,19 +1545,19 @@
       <c r="V6">
         <v>0.97</v>
       </c>
-      <c r="Z6" s="7" t="s">
+      <c r="Z6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="AA6" s="8"/>
-      <c r="AB6" s="9" t="s">
+      <c r="AA6" s="24"/>
+      <c r="AB6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="AC6" s="3"/>
-      <c r="AD6" s="3"/>
-      <c r="AE6" s="3"/>
-      <c r="AF6" s="3"/>
-      <c r="AG6" s="3"/>
-      <c r="AH6" s="3"/>
+      <c r="AC6" s="19"/>
+      <c r="AD6" s="19"/>
+      <c r="AE6" s="19"/>
+      <c r="AF6" s="19"/>
+      <c r="AG6" s="19"/>
+      <c r="AH6" s="19"/>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1623,31 +1623,31 @@
       <c r="Y7" t="s">
         <v>10</v>
       </c>
-      <c r="Z7" s="7">
+      <c r="Z7" s="5">
         <v>0.66</v>
       </c>
-      <c r="AA7" s="10">
+      <c r="AA7" s="7">
         <v>0.31</v>
       </c>
-      <c r="AB7" s="9">
+      <c r="AB7" s="6">
         <v>0.03</v>
       </c>
-      <c r="AC7" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD7" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AE7" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF7" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG7" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH7" s="3" t="s">
+      <c r="AC7" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD7" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE7" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF7" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG7" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH7" s="19" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1712,21 +1712,21 @@
       <c r="V8">
         <v>0.97</v>
       </c>
-      <c r="Z8" s="7" t="s">
+      <c r="Z8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="AA8" s="10" t="s">
+      <c r="AA8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="AB8" s="9" t="s">
+      <c r="AB8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="AC8" s="3"/>
-      <c r="AD8" s="3"/>
-      <c r="AE8" s="3"/>
-      <c r="AF8" s="3"/>
-      <c r="AG8" s="3"/>
-      <c r="AH8" s="3"/>
+      <c r="AC8" s="19"/>
+      <c r="AD8" s="19"/>
+      <c r="AE8" s="19"/>
+      <c r="AF8" s="19"/>
+      <c r="AG8" s="19"/>
+      <c r="AH8" s="19"/>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1792,31 +1792,31 @@
       <c r="Y9" t="s">
         <v>11</v>
       </c>
-      <c r="Z9" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA9" s="10">
+      <c r="Z9" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA9" s="7">
         <v>0.1</v>
       </c>
-      <c r="AB9" s="9">
+      <c r="AB9" s="6">
         <v>0.8</v>
       </c>
-      <c r="AC9" s="4">
+      <c r="AC9" s="2">
         <v>0.09</v>
       </c>
-      <c r="AD9" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AE9" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF9" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG9" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH9" s="3" t="s">
+      <c r="AD9" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE9" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF9" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG9" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH9" s="19" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1881,21 +1881,21 @@
       <c r="V10">
         <v>0.54</v>
       </c>
-      <c r="Z10" s="12"/>
-      <c r="AA10" s="13" t="s">
+      <c r="Z10" s="23"/>
+      <c r="AA10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="AB10" s="14" t="s">
+      <c r="AB10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="AC10" s="4" t="s">
+      <c r="AC10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AD10" s="3"/>
-      <c r="AE10" s="3"/>
-      <c r="AF10" s="3"/>
-      <c r="AG10" s="3"/>
-      <c r="AH10" s="3"/>
+      <c r="AD10" s="19"/>
+      <c r="AE10" s="19"/>
+      <c r="AF10" s="19"/>
+      <c r="AG10" s="19"/>
+      <c r="AH10" s="19"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1961,31 +1961,31 @@
       <c r="Y11" t="s">
         <v>12</v>
       </c>
-      <c r="Z11" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA11" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB11" s="4">
+      <c r="Z11" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA11" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB11" s="2">
         <v>0.01</v>
       </c>
-      <c r="AC11" s="15">
+      <c r="AC11" s="10">
         <v>0.92</v>
       </c>
-      <c r="AD11" s="4">
+      <c r="AD11" s="2">
         <v>0.01</v>
       </c>
-      <c r="AE11" s="4">
+      <c r="AE11" s="2">
         <v>0.01</v>
       </c>
-      <c r="AF11" s="4">
+      <c r="AF11" s="2">
         <v>0.05</v>
       </c>
-      <c r="AG11" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH11" s="3" t="s">
+      <c r="AG11" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH11" s="19" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2050,64 +2050,64 @@
       <c r="V12">
         <v>0.8</v>
       </c>
-      <c r="Z12" s="3"/>
-      <c r="AA12" s="3"/>
-      <c r="AB12" s="4" t="s">
+      <c r="Z12" s="19"/>
+      <c r="AA12" s="19"/>
+      <c r="AB12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC12" s="16" t="s">
+      <c r="AC12" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AD12" s="4" t="s">
+      <c r="AD12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AE12" s="4" t="s">
+      <c r="AE12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AF12" s="4" t="s">
+      <c r="AF12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AG12" s="3"/>
-      <c r="AH12" s="3"/>
+      <c r="AG12" s="19"/>
+      <c r="AH12" s="19"/>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="22">
-        <v>0</v>
-      </c>
-      <c r="C13" s="22">
+      <c r="B13" s="15">
+        <v>0</v>
+      </c>
+      <c r="C13" s="15">
         <v>6</v>
       </c>
-      <c r="D13" s="22">
-        <v>0</v>
-      </c>
-      <c r="E13" s="22">
+      <c r="D13" s="15">
+        <v>0</v>
+      </c>
+      <c r="E13" s="15">
         <v>1</v>
       </c>
-      <c r="F13" s="22">
-        <v>0</v>
-      </c>
-      <c r="G13" s="22">
-        <v>0</v>
-      </c>
-      <c r="H13" s="22">
-        <v>0</v>
-      </c>
-      <c r="I13" s="22">
-        <v>0</v>
-      </c>
-      <c r="J13" s="22">
-        <v>0</v>
-      </c>
-      <c r="K13" s="22">
-        <v>0</v>
-      </c>
-      <c r="L13" s="22">
-        <v>0</v>
-      </c>
-      <c r="M13" s="22">
+      <c r="F13" s="15">
+        <v>0</v>
+      </c>
+      <c r="G13" s="15">
+        <v>0</v>
+      </c>
+      <c r="H13" s="15">
+        <v>0</v>
+      </c>
+      <c r="I13" s="15">
+        <v>0</v>
+      </c>
+      <c r="J13" s="15">
+        <v>0</v>
+      </c>
+      <c r="K13" s="15">
+        <v>0</v>
+      </c>
+      <c r="L13" s="15">
+        <v>0</v>
+      </c>
+      <c r="M13" s="15">
         <v>0</v>
       </c>
       <c r="O13" t="s">
@@ -2134,29 +2134,29 @@
       <c r="Y13" t="s">
         <v>13</v>
       </c>
-      <c r="Z13" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA13" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB13" s="4"/>
-      <c r="AC13" s="4">
+      <c r="Z13" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA13" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2">
         <v>0.04</v>
       </c>
-      <c r="AD13" s="5">
+      <c r="AD13" s="3">
         <v>0.6</v>
       </c>
-      <c r="AE13" s="17">
+      <c r="AE13" s="12">
         <v>0.26</v>
       </c>
-      <c r="AF13" s="6">
+      <c r="AF13" s="4">
         <v>0.09</v>
       </c>
-      <c r="AG13" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH13" s="3" t="s">
+      <c r="AG13" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH13" s="19" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2182,78 +2182,78 @@
       <c r="V14">
         <v>0.81</v>
       </c>
-      <c r="Z14" s="3"/>
-      <c r="AA14" s="3"/>
-      <c r="AB14" s="4"/>
-      <c r="AC14" s="4" t="s">
+      <c r="Z14" s="19"/>
+      <c r="AA14" s="19"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AD14" s="7" t="s">
+      <c r="AD14" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AE14" s="10" t="s">
+      <c r="AE14" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AF14" s="9" t="s">
+      <c r="AF14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AG14" s="3"/>
-      <c r="AH14" s="3"/>
+      <c r="AG14" s="19"/>
+      <c r="AH14" s="19"/>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>64</v>
       </c>
-      <c r="O15" s="23" t="s">
+      <c r="O15" s="16" t="s">
         <v>34</v>
       </c>
       <c r="Y15" t="s">
         <v>14</v>
       </c>
-      <c r="Z15" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA15" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB15" s="4">
+      <c r="Z15" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA15" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB15" s="2">
         <v>0.01</v>
       </c>
-      <c r="AC15" s="4">
+      <c r="AC15" s="2">
         <v>0.22</v>
       </c>
-      <c r="AD15" s="7">
+      <c r="AD15" s="5">
         <v>0.17</v>
       </c>
-      <c r="AE15" s="10">
+      <c r="AE15" s="7">
         <v>0.41</v>
       </c>
-      <c r="AF15" s="9">
+      <c r="AF15" s="6">
         <v>0.17</v>
       </c>
-      <c r="AG15" s="4">
+      <c r="AG15" s="2">
         <v>0.01</v>
       </c>
-      <c r="AH15" s="3" t="s">
+      <c r="AH15" s="19" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21" t="s">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
       <c r="O16" t="s">
         <v>35</v>
       </c>
@@ -2275,66 +2275,66 @@
       <c r="V16">
         <v>0.98</v>
       </c>
-      <c r="Z16" s="3"/>
-      <c r="AA16" s="3"/>
-      <c r="AB16" s="4" t="s">
+      <c r="Z16" s="19"/>
+      <c r="AA16" s="19"/>
+      <c r="AB16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AC16" s="4" t="s">
+      <c r="AC16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AD16" s="7" t="s">
+      <c r="AD16" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AE16" s="10" t="s">
+      <c r="AE16" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="AF16" s="9" t="s">
+      <c r="AF16" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="AG16" s="4" t="s">
+      <c r="AG16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AH16" s="3"/>
+      <c r="AH16" s="19"/>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="F17" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="22" t="s">
+      <c r="G17" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="22" t="s">
+      <c r="H17" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="I17" s="22" t="s">
+      <c r="I17" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="J17" s="22" t="s">
+      <c r="J17" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="K17" s="22" t="s">
+      <c r="K17" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="L17" s="22" t="s">
+      <c r="L17" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="M17" s="22" t="s">
+      <c r="M17" s="15" t="s">
         <v>59</v>
       </c>
       <c r="O17" t="s">
@@ -2361,31 +2361,31 @@
       <c r="Y17" t="s">
         <v>15</v>
       </c>
-      <c r="Z17" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA17" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB17" s="4">
+      <c r="Z17" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA17" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB17" s="2">
         <v>0.02</v>
       </c>
-      <c r="AC17" s="4">
+      <c r="AC17" s="2">
         <v>0.13</v>
       </c>
-      <c r="AD17" s="7">
+      <c r="AD17" s="5">
         <v>0.02</v>
       </c>
-      <c r="AE17" s="10">
+      <c r="AE17" s="7">
         <v>0.34</v>
       </c>
-      <c r="AF17" s="9">
+      <c r="AF17" s="6">
         <v>0.47</v>
       </c>
-      <c r="AG17" s="4">
+      <c r="AG17" s="2">
         <v>0.01</v>
       </c>
-      <c r="AH17" s="3" t="s">
+      <c r="AH17" s="19" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2450,27 +2450,27 @@
       <c r="V18">
         <v>0.72</v>
       </c>
-      <c r="Z18" s="3"/>
-      <c r="AA18" s="3"/>
-      <c r="AB18" s="4" t="s">
+      <c r="Z18" s="19"/>
+      <c r="AA18" s="19"/>
+      <c r="AB18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AC18" s="4" t="s">
+      <c r="AC18" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AD18" s="18" t="s">
+      <c r="AD18" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="AE18" s="13" t="s">
+      <c r="AE18" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="AF18" s="14" t="s">
+      <c r="AF18" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="AG18" s="4" t="s">
+      <c r="AG18" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AH18" s="3"/>
+      <c r="AH18" s="19"/>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -2536,31 +2536,31 @@
       <c r="Y19" t="s">
         <v>16</v>
       </c>
-      <c r="Z19" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA19" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB19" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC19" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD19" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AE19" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF19" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG19" s="5">
+      <c r="Z19" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA19" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB19" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC19" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD19" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE19" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF19" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG19" s="3">
         <v>1</v>
       </c>
-      <c r="AH19" s="19" t="s">
+      <c r="AH19" s="20" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2604,33 +2604,33 @@
       <c r="M20">
         <v>0</v>
       </c>
-      <c r="O20" s="22" t="s">
+      <c r="O20" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="22"/>
-      <c r="R20" s="22"/>
-      <c r="S20" s="22"/>
-      <c r="T20" s="22">
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15">
         <v>0.73</v>
       </c>
-      <c r="U20" s="22">
+      <c r="U20" s="15">
         <v>0.69</v>
       </c>
-      <c r="V20" s="22">
+      <c r="V20" s="15">
         <v>0.76</v>
       </c>
-      <c r="Z20" s="3"/>
-      <c r="AA20" s="3"/>
-      <c r="AB20" s="3"/>
-      <c r="AC20" s="3"/>
-      <c r="AD20" s="3"/>
-      <c r="AE20" s="3"/>
-      <c r="AF20" s="3"/>
-      <c r="AG20" s="7" t="s">
+      <c r="Z20" s="19"/>
+      <c r="AA20" s="19"/>
+      <c r="AB20" s="19"/>
+      <c r="AC20" s="19"/>
+      <c r="AD20" s="19"/>
+      <c r="AE20" s="19"/>
+      <c r="AF20" s="19"/>
+      <c r="AG20" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="AH20" s="20"/>
+      <c r="AH20" s="21"/>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -2675,31 +2675,31 @@
       <c r="Y21" t="s">
         <v>17</v>
       </c>
-      <c r="Z21" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA21" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB21" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC21" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD21" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AE21" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF21" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG21" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH21" s="9">
+      <c r="Z21" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA21" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB21" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC21" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD21" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE21" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF21" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG21" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH21" s="6">
         <v>1</v>
       </c>
     </row>
@@ -2743,15 +2743,15 @@
       <c r="M22">
         <v>14</v>
       </c>
-      <c r="Z22" s="3"/>
-      <c r="AA22" s="3"/>
-      <c r="AB22" s="3"/>
-      <c r="AC22" s="3"/>
-      <c r="AD22" s="3"/>
-      <c r="AE22" s="3"/>
-      <c r="AF22" s="3"/>
-      <c r="AG22" s="12"/>
-      <c r="AH22" s="14" t="s">
+      <c r="Z22" s="19"/>
+      <c r="AA22" s="19"/>
+      <c r="AB22" s="19"/>
+      <c r="AC22" s="19"/>
+      <c r="AD22" s="19"/>
+      <c r="AE22" s="19"/>
+      <c r="AF22" s="19"/>
+      <c r="AG22" s="23"/>
+      <c r="AH22" s="9" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2879,43 +2879,43 @@
       </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="22">
-        <v>0</v>
-      </c>
-      <c r="C26" s="22">
-        <v>0</v>
-      </c>
-      <c r="D26" s="22">
+      <c r="B26" s="15">
+        <v>0</v>
+      </c>
+      <c r="C26" s="15">
+        <v>0</v>
+      </c>
+      <c r="D26" s="15">
         <v>5</v>
       </c>
-      <c r="E26" s="22">
+      <c r="E26" s="15">
         <v>1</v>
       </c>
-      <c r="F26" s="22">
+      <c r="F26" s="15">
         <v>5</v>
       </c>
-      <c r="G26" s="22">
+      <c r="G26" s="15">
         <v>3</v>
       </c>
-      <c r="H26" s="22">
+      <c r="H26" s="15">
         <v>4</v>
       </c>
-      <c r="I26" s="22">
+      <c r="I26" s="15">
         <v>1</v>
       </c>
-      <c r="J26" s="22">
+      <c r="J26" s="15">
         <v>1</v>
       </c>
-      <c r="K26" s="22">
-        <v>0</v>
-      </c>
-      <c r="L26" s="22">
-        <v>0</v>
-      </c>
-      <c r="M26" s="22">
+      <c r="K26" s="15">
+        <v>0</v>
+      </c>
+      <c r="L26" s="15">
+        <v>0</v>
+      </c>
+      <c r="M26" s="15">
         <v>0</v>
       </c>
     </row>
@@ -2925,60 +2925,60 @@
       </c>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21" t="s">
+      <c r="A29" s="14"/>
+      <c r="B29" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="21"/>
-      <c r="M29" s="21"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D30" s="22" t="s">
+      <c r="D30" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="E30" s="22" t="s">
+      <c r="E30" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="F30" s="22" t="s">
+      <c r="F30" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="G30" s="22" t="s">
+      <c r="G30" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="H30" s="22" t="s">
+      <c r="H30" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="I30" s="22" t="s">
+      <c r="I30" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="J30" s="22" t="s">
+      <c r="J30" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="K30" s="22" t="s">
+      <c r="K30" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="L30" s="22" t="s">
+      <c r="L30" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="M30" s="22" t="s">
+      <c r="M30" s="15" t="s">
         <v>59</v>
       </c>
     </row>
@@ -3311,57 +3311,74 @@
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="22" t="s">
+      <c r="A39" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B39" s="24" t="s">
+      <c r="B39" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="24">
-        <v>0</v>
-      </c>
-      <c r="D39" s="24">
+      <c r="C39" s="17">
+        <v>0</v>
+      </c>
+      <c r="D39" s="17">
         <v>0.83333333333333304</v>
       </c>
-      <c r="E39" s="24">
+      <c r="E39" s="17">
         <v>0.14285714285714299</v>
       </c>
-      <c r="F39" s="24">
+      <c r="F39" s="17">
         <v>0.71428571428571397</v>
       </c>
-      <c r="G39" s="24">
+      <c r="G39" s="17">
         <v>0.42857142857142899</v>
       </c>
-      <c r="H39" s="24">
+      <c r="H39" s="17">
         <v>0.57142857142857095</v>
       </c>
-      <c r="I39" s="24">
+      <c r="I39" s="17">
         <v>0.14285714285714299</v>
       </c>
-      <c r="J39" s="24">
+      <c r="J39" s="17">
         <v>0.14285714285714299</v>
       </c>
-      <c r="K39" s="24">
-        <v>0</v>
-      </c>
-      <c r="L39" s="24">
-        <v>0</v>
-      </c>
-      <c r="M39" s="24">
+      <c r="K39" s="17">
+        <v>0</v>
+      </c>
+      <c r="L39" s="17">
+        <v>0</v>
+      </c>
+      <c r="M39" s="17">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="AH15:AH16"/>
-    <mergeCell ref="AH17:AH18"/>
-    <mergeCell ref="AH19:AH20"/>
-    <mergeCell ref="AG13:AG14"/>
-    <mergeCell ref="AH5:AH6"/>
-    <mergeCell ref="AH7:AH8"/>
-    <mergeCell ref="AH9:AH10"/>
-    <mergeCell ref="AH11:AH12"/>
-    <mergeCell ref="AH13:AH14"/>
+    <mergeCell ref="O1:V2"/>
+    <mergeCell ref="Y1:AH2"/>
+    <mergeCell ref="Z9:Z10"/>
+    <mergeCell ref="Z11:Z12"/>
+    <mergeCell ref="Z13:Z14"/>
+    <mergeCell ref="AG5:AG6"/>
+    <mergeCell ref="AG7:AG8"/>
+    <mergeCell ref="AG9:AG10"/>
+    <mergeCell ref="AG11:AG12"/>
+    <mergeCell ref="Z15:Z16"/>
+    <mergeCell ref="Z17:Z18"/>
+    <mergeCell ref="Z19:Z20"/>
+    <mergeCell ref="Z21:Z22"/>
+    <mergeCell ref="AA5:AA6"/>
+    <mergeCell ref="AA11:AA12"/>
+    <mergeCell ref="AA13:AA14"/>
+    <mergeCell ref="AA15:AA16"/>
+    <mergeCell ref="AA17:AA18"/>
+    <mergeCell ref="AA19:AA20"/>
+    <mergeCell ref="AA21:AA22"/>
+    <mergeCell ref="AC5:AC6"/>
+    <mergeCell ref="AC7:AC8"/>
+    <mergeCell ref="AB19:AB20"/>
+    <mergeCell ref="AB21:AB22"/>
+    <mergeCell ref="AC19:AC20"/>
+    <mergeCell ref="AC21:AC22"/>
     <mergeCell ref="AG21:AG22"/>
     <mergeCell ref="AD5:AD6"/>
     <mergeCell ref="AD7:AD8"/>
@@ -3378,32 +3395,15 @@
     <mergeCell ref="AE21:AE22"/>
     <mergeCell ref="AF19:AF20"/>
     <mergeCell ref="AF21:AF22"/>
-    <mergeCell ref="AA21:AA22"/>
-    <mergeCell ref="AC5:AC6"/>
-    <mergeCell ref="AC7:AC8"/>
-    <mergeCell ref="AB19:AB20"/>
-    <mergeCell ref="AB21:AB22"/>
-    <mergeCell ref="AC19:AC20"/>
-    <mergeCell ref="AC21:AC22"/>
-    <mergeCell ref="Z15:Z16"/>
-    <mergeCell ref="Z17:Z18"/>
-    <mergeCell ref="Z19:Z20"/>
-    <mergeCell ref="Z21:Z22"/>
-    <mergeCell ref="AA5:AA6"/>
-    <mergeCell ref="AA11:AA12"/>
-    <mergeCell ref="AA13:AA14"/>
-    <mergeCell ref="AA15:AA16"/>
-    <mergeCell ref="AA17:AA18"/>
-    <mergeCell ref="AA19:AA20"/>
-    <mergeCell ref="O1:V2"/>
-    <mergeCell ref="Y1:AH2"/>
-    <mergeCell ref="Z9:Z10"/>
-    <mergeCell ref="Z11:Z12"/>
-    <mergeCell ref="Z13:Z14"/>
-    <mergeCell ref="AG5:AG6"/>
-    <mergeCell ref="AG7:AG8"/>
-    <mergeCell ref="AG9:AG10"/>
-    <mergeCell ref="AG11:AG12"/>
+    <mergeCell ref="AH15:AH16"/>
+    <mergeCell ref="AH17:AH18"/>
+    <mergeCell ref="AH19:AH20"/>
+    <mergeCell ref="AG13:AG14"/>
+    <mergeCell ref="AH5:AH6"/>
+    <mergeCell ref="AH7:AH8"/>
+    <mergeCell ref="AH9:AH10"/>
+    <mergeCell ref="AH11:AH12"/>
+    <mergeCell ref="AH13:AH14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>